<commit_message>
Started loading dose form. Failed due to encoding. Moved folder from documents to Docs. Hard coded paths may be corrupt
</commit_message>
<xml_diff>
--- a/unit_mapping/man_map_unit_strength.xlsx
+++ b/unit_mapping/man_map_unit_strength.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maxim/Documents/Drug_mapping_OHDSI/unit_mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maxim/Google Drive/Bedrijf/Projects/Janssen-OHDSI AUH/Execution/Drug_Mapping_Scripts/unit_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="171">
   <si>
     <t xml:space="preserve"> strunut </t>
   </si>
@@ -534,13 +534,19 @@
   </si>
   <si>
     <t>geen idee hoe een ratio weer te geven in drug_strength</t>
+  </si>
+  <si>
+    <t>volume percent</t>
+  </si>
+  <si>
+    <t>weight percent weight</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -565,6 +571,22 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -593,8 +615,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -614,10 +642,35 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -625,6 +678,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H1048576" totalsRowShown="0">
+  <autoFilter ref="A1:H1048576"/>
+  <sortState ref="A2:H64">
+    <sortCondition ref="A1:A1048576"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" name=" strunut "/>
+    <tableColumn id="2" name="       streng        " dataDxfId="2"/>
+    <tableColumn id="3" name="Frequency" dataDxfId="1"/>
+    <tableColumn id="4" name="Remark" dataDxfId="0"/>
+    <tableColumn id="5" name="concept_id"/>
+    <tableColumn id="6" name="concept_name"/>
+    <tableColumn id="7" name="num_concept_id"/>
+    <tableColumn id="8" name="denom_concept_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -892,20 +965,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -936,21 +1010,18 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="C2" s="7">
-        <v>1</v>
+        <v>7024</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -958,240 +1029,225 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7">
         <v>9</v>
-      </c>
-      <c r="C5" s="7">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7">
         <v>11</v>
-      </c>
-      <c r="C6" s="7">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="7">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="7">
-        <v>458</v>
-      </c>
-      <c r="E8" s="1">
-        <v>8504</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>125</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7">
-        <v>6</v>
+        <v>458</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8504</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="7">
-        <v>83</v>
-      </c>
-      <c r="E10" s="1">
-        <v>8636</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="7">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="E11" s="1">
-        <v>9514</v>
+        <v>8636</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9514</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="7">
-        <v>371</v>
-      </c>
-      <c r="E15" s="1">
-        <v>8718</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>154</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1">
+        <v>371</v>
+      </c>
+      <c r="E16" s="1">
         <v>8718</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="7">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1">
-        <v>9333</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>155</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1">
         <v>8718</v>
       </c>
-      <c r="H17" s="1">
-        <v>8504</v>
-      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="7">
-        <v>486</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1">
-        <v>8985</v>
+        <v>9333</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G18" s="1">
         <v>8718</v>
       </c>
       <c r="H18" s="1">
-        <v>8587</v>
+        <v>8504</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="7">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>157</v>
+        <v>486</v>
       </c>
       <c r="E19" s="1">
-        <v>9525</v>
+        <v>8985</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G19" s="6">
+        <v>156</v>
+      </c>
+      <c r="G19" s="1">
         <v>8718</v>
       </c>
       <c r="H19" s="1">
@@ -1200,70 +1256,76 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="7">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="1">
+        <v>9525</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G20" s="6">
+        <v>8718</v>
+      </c>
+      <c r="H20" s="1">
+        <v>8587</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="7">
-        <v>18773</v>
-      </c>
-      <c r="E21" s="1">
-        <v>8576</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="7">
-        <v>2</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>136</v>
+        <v>18773</v>
       </c>
       <c r="E22" s="1">
-        <v>9564</v>
+        <v>8576</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G22" s="1">
-        <v>8576</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="7">
-        <v>211</v>
+        <v>2</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="E23" s="1">
-        <v>45890997</v>
+        <v>9564</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G23" s="1">
         <v>8576</v>
@@ -1271,22 +1333,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="7">
-        <v>2</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="E24" s="1">
-        <v>45891022</v>
+        <v>45890997</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G24" s="1">
         <v>8576</v>
@@ -1294,706 +1353,744 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="7">
-        <v>498</v>
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="E25" s="1">
-        <v>8723</v>
+        <v>45891022</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G25" s="1">
         <v>8576</v>
       </c>
-      <c r="H25" s="1">
-        <v>8504</v>
-      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="7">
-        <v>102</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>133</v>
+        <v>498</v>
       </c>
       <c r="E26" s="1">
-        <v>8909</v>
+        <v>8723</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G26" s="1">
         <v>8576</v>
       </c>
-      <c r="H26" s="2">
-        <v>8512</v>
+      <c r="H26" s="1">
+        <v>8504</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="7">
-        <v>4</v>
+        <v>102</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="E27" s="1">
-        <v>45891036</v>
+        <v>8909</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G27" s="1">
         <v>8576</v>
       </c>
       <c r="H27" s="2">
-        <v>9483</v>
+        <v>8512</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="7">
         <v>4</v>
       </c>
       <c r="E28" s="1">
-        <v>8751</v>
+        <v>45891036</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G28" s="1">
         <v>8576</v>
       </c>
       <c r="H28" s="2">
-        <v>8519</v>
+        <v>9483</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" s="7">
-        <v>4797</v>
+        <v>4</v>
       </c>
       <c r="E29" s="1">
-        <v>8861</v>
+        <v>8751</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G29" s="1">
         <v>8576</v>
       </c>
-      <c r="H29" s="1">
-        <v>8587</v>
+      <c r="H29" s="2">
+        <v>8519</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" s="7">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>133</v>
+        <v>4797</v>
       </c>
       <c r="E30" s="1">
-        <v>45891021</v>
+        <v>8861</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G30" s="1">
         <v>8576</v>
       </c>
+      <c r="H30" s="1">
+        <v>8587</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>133</v>
       </c>
       <c r="E31" s="1">
-        <v>9040</v>
+        <v>45891021</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="G31" s="1">
-        <v>44777577</v>
-      </c>
-      <c r="H31" s="2">
-        <v>8519</v>
+        <v>8576</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="7">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="E32" s="1">
-        <v>9550</v>
+        <v>9040</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G32" s="1">
         <v>44777577</v>
       </c>
-      <c r="H32" s="1">
-        <v>8587</v>
+      <c r="H32" s="2">
+        <v>8519</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" s="7">
-        <v>138</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1">
+        <v>9550</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="1">
         <v>44777577</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G33" s="1"/>
+      <c r="H33" s="1">
+        <v>8587</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="7">
-        <v>338</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E34" s="1">
+        <v>44777577</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="7">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1">
-        <v>8587</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>142</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="7">
         <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>8753</v>
+        <v>8587</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" s="2">
-        <v>9573</v>
-      </c>
-      <c r="H36" s="2">
-        <v>8519</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C37" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1">
+        <v>8753</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" s="2">
         <v>9573</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>162</v>
+      <c r="H37" s="2">
+        <v>8519</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38" s="7">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="E38" s="1">
-        <v>45891014</v>
+        <v>9573</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="2">
-        <v>9573</v>
-      </c>
-      <c r="H38" s="1">
-        <v>8587</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="8">
-        <v>5.0000000000000001E-4</v>
+        <v>74</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="C39" s="7">
-        <v>1433</v>
-      </c>
-      <c r="D39" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="E39" s="1">
+        <v>45891014</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G39" s="2">
+        <v>9573</v>
+      </c>
+      <c r="H39" s="1">
+        <v>8587</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="B40" s="8">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C40" s="7">
-        <v>7</v>
+        <v>1433</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="1">
+        <v>8554</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="9">
-        <v>0.25</v>
+        <v>77</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C41" s="7">
-        <v>14</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="1">
-        <v>8554</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>163</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0.25</v>
       </c>
       <c r="C42" s="7">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="1">
+        <v>8554</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C43" s="7">
-        <v>4</v>
-      </c>
-      <c r="E43" s="1">
-        <v>9387</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>153</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="9">
-        <v>0.2</v>
+        <v>82</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="C44" s="7">
-        <v>20</v>
-      </c>
-      <c r="D44" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
+        <v>9387</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" s="9">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="C45" s="7">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D45" s="5"/>
+      <c r="E45" s="1">
+        <v>9234</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="B46" s="9">
+        <v>0.08</v>
       </c>
       <c r="C46" s="7">
-        <v>512</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D46" s="5"/>
       <c r="E46" s="1">
-        <v>9655</v>
+        <v>45891011</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C47" s="7">
-        <v>455</v>
+        <v>512</v>
       </c>
       <c r="E47" s="1">
-        <v>45890998</v>
+        <v>9655</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G47" s="1">
-        <v>9655</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" s="7">
-        <v>39</v>
+        <v>455</v>
       </c>
       <c r="E48" s="1">
-        <v>8720</v>
+        <v>45890998</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G48" s="1">
         <v>9655</v>
       </c>
-      <c r="H48" s="1">
-        <v>8504</v>
-      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="7">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E49" s="1">
-        <v>8906</v>
+        <v>8720</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G49" s="1">
         <v>9655</v>
       </c>
-      <c r="H49" s="2">
-        <v>8512</v>
+      <c r="H49" s="1">
+        <v>8504</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C50" s="7">
-        <v>227</v>
+        <v>67</v>
       </c>
       <c r="E50" s="1">
-        <v>8859</v>
+        <v>8906</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G50" s="1">
         <v>9655</v>
       </c>
-      <c r="H50" s="1">
-        <v>8587</v>
+      <c r="H50" s="2">
+        <v>8512</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C51" s="7">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="E51" s="1">
-        <v>44777645</v>
+        <v>8859</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G51" s="1">
         <v>9655</v>
       </c>
-      <c r="H51" s="2">
-        <v>8505</v>
+      <c r="H51" s="1">
+        <v>8587</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C52" s="7">
-        <v>2</v>
+        <v>144</v>
+      </c>
+      <c r="E52" s="1">
+        <v>44777645</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G52" s="1">
+        <v>9655</v>
+      </c>
+      <c r="H52" s="2">
+        <v>8505</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C53" s="7">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1">
-        <v>45891029</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G53" s="2">
-        <v>9665</v>
-      </c>
-      <c r="H53" s="1">
-        <v>8587</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C54" s="7">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <v>45891029</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G54" s="2">
+        <v>9665</v>
+      </c>
+      <c r="H54" s="1">
+        <v>8587</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C55" s="7">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C56" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C57" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C58" s="7">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C59" s="7">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C60" s="7">
-        <v>65</v>
-      </c>
-      <c r="E60" s="1">
-        <v>8763</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G60" s="1">
-        <v>8510</v>
-      </c>
-      <c r="H60" s="1">
-        <v>8587</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C61" s="7">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E61" s="1">
+        <v>8763</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G61" s="1">
         <v>8510</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>164</v>
+      <c r="H61" s="1">
+        <v>8587</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" s="7">
-        <v>108</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>168</v>
+        <v>35</v>
       </c>
       <c r="E62" s="1">
-        <v>8523</v>
+        <v>8510</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C63" s="7">
-        <v>133</v>
+        <v>108</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E63" s="1">
+        <v>8523</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="C64" s="7">
-        <v>7024</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added function converting strength string to number. Changed input to new auh products from lars. No need for druglist anymore.
</commit_message>
<xml_diff>
--- a/unit_mapping/man_map_unit_strength.xlsx
+++ b/unit_mapping/man_map_unit_strength.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22160" tabRatio="500"/>
+    <workbookView xWindow="12100" yWindow="800" windowWidth="38400" windowHeight="22160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
   <si>
     <t xml:space="preserve"> strunut </t>
   </si>
@@ -533,13 +533,19 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>geen idee hoe een ratio weer te geven in drug_strength</t>
-  </si>
-  <si>
     <t>volume percent</t>
   </si>
   <si>
     <t>weight percent weight</t>
+  </si>
+  <si>
+    <t>Ehrlich unit per milliliter</t>
+  </si>
+  <si>
+    <t>plaque forming unit</t>
+  </si>
+  <si>
+    <t>In nieuwe dataset Lars wordt dit naar fractie omgerekend</t>
   </si>
 </sst>
 </file>
@@ -966,8 +972,8 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46:F46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,6 +1087,12 @@
       <c r="C8" s="7">
         <v>17</v>
       </c>
+      <c r="E8" s="1">
+        <v>8695</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1732,6 +1744,12 @@
       <c r="C43" s="7">
         <v>1</v>
       </c>
+      <c r="E43" s="1">
+        <v>9379</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1765,7 +1783,7 @@
         <v>9234</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1783,7 +1801,7 @@
         <v>45891011</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2066,7 +2084,7 @@
         <v>108</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E63" s="1">
         <v>8523</v>

</xml_diff>

<commit_message>
First version of final mapping script. Moved mapping files to seperate folder
</commit_message>
<xml_diff>
--- a/unit_mapping/man_map_unit_strength.xlsx
+++ b/unit_mapping/man_map_unit_strength.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="800" windowWidth="38400" windowHeight="22160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="174">
   <si>
     <t xml:space="preserve"> strunut </t>
   </si>
@@ -35,363 +35,177 @@
     <t xml:space="preserve">       streng        </t>
   </si>
   <si>
-    <t xml:space="preserve"> AUM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 50 AMU</t>
   </si>
   <si>
-    <t xml:space="preserve"> BAB     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2 Mia bakterier</t>
   </si>
   <si>
-    <t xml:space="preserve"> BHS     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> BehandlingssÃ¦t</t>
   </si>
   <si>
-    <t xml:space="preserve"> EID     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1000 E.I.D.</t>
   </si>
   <si>
-    <t xml:space="preserve"> EP      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Lipase 25.000 EP-e</t>
   </si>
   <si>
-    <t xml:space="preserve"> EUM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1440 EU/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> G       </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 G</t>
   </si>
   <si>
-    <t xml:space="preserve"> GDO     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 g</t>
   </si>
   <si>
-    <t xml:space="preserve"> GL      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100 G/L</t>
   </si>
   <si>
-    <t xml:space="preserve"> GML     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 g/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> HEP     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10 HEP</t>
   </si>
   <si>
-    <t xml:space="preserve"> HT      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 250 mg</t>
   </si>
   <si>
-    <t xml:space="preserve"> INS     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> InitialsÃ¦t</t>
   </si>
   <si>
-    <t xml:space="preserve"> IU      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1000 IE</t>
   </si>
   <si>
-    <t xml:space="preserve"> IUD     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 200 IE/dosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> IUG     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100.000 IE/g</t>
   </si>
   <si>
-    <t xml:space="preserve"> IUM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 320.000 IE/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> KIM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10.000 KIE/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> MEM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 30 mill. E/0,5 ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> MG      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 75 mg</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGC     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0,52 mg/cm</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGD     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0,5 mg/dosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGF     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 mg/72 timer</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGG     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2,5 mg/g</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGH     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8 mg/24 timer</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGK     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1,3 mg/cm2</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGL     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 200 mg/l</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 6 mg/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> MGS     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 25 mg/16 timer</t>
   </si>
   <si>
-    <t xml:space="preserve"> MIL     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 7,77 Mill E</t>
   </si>
   <si>
-    <t xml:space="preserve"> MIM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 4,5 Mill. IE/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> MIU     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 Mill. IE</t>
   </si>
   <si>
-    <t xml:space="preserve"> MJM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 350 mg jod/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> ML      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 ml/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> MML     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2 mmol/l</t>
   </si>
   <si>
-    <t xml:space="preserve"> MMO     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 6 mmol Li+</t>
   </si>
   <si>
-    <t xml:space="preserve"> MOM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0,15 mmol/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> PC      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PDO     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100.000 pfu/dosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> PER     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PFU     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2000 PFU</t>
   </si>
   <si>
-    <t xml:space="preserve"> PPM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 450 ppm</t>
   </si>
   <si>
-    <t xml:space="preserve"> PV      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PW      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RG      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 130 mikrogram</t>
   </si>
   <si>
-    <t xml:space="preserve"> RGD     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100 mikg/dosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> RGG     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 500 mikrogram/g</t>
   </si>
   <si>
-    <t xml:space="preserve"> RGH     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 50 mikg/24 timer</t>
   </si>
   <si>
-    <t xml:space="preserve"> RGM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 20 mikrogram/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> RGT     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100 mikrogram/time</t>
   </si>
   <si>
-    <t xml:space="preserve"> RGV     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 120 mikg/htgl.</t>
   </si>
   <si>
-    <t xml:space="preserve"> RLM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8 mikroliter/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> SQ      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 75.000 SQ.T</t>
   </si>
   <si>
-    <t xml:space="preserve"> SQM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10.000 sq-u/ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> SQV     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1.000.000 sq-u/htgl</t>
   </si>
   <si>
-    <t xml:space="preserve"> ST      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 750 mg</t>
   </si>
   <si>
-    <t xml:space="preserve"> TCI     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10.000 TCID50/dosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> UDO     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2 TE/dosis</t>
   </si>
   <si>
-    <t xml:space="preserve"> UML     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10.000 enh./ml</t>
   </si>
   <si>
-    <t xml:space="preserve"> UN      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100 enheder</t>
   </si>
   <si>
-    <t xml:space="preserve"> WV      </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1:100 W/V</t>
   </si>
   <si>
-    <t xml:space="preserve"> XAM     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2.500 anti-Xa IE/ml</t>
   </si>
   <si>
@@ -530,9 +344,6 @@
     <t>ratio</t>
   </si>
   <si>
-    <t>Frequency</t>
-  </si>
-  <si>
     <t>volume percent</t>
   </si>
   <si>
@@ -545,7 +356,199 @@
     <t>plaque forming unit</t>
   </si>
   <si>
-    <t>In nieuwe dataset Lars wordt dit naar fractie omgerekend</t>
+    <t>Frequency2</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>of unit: 8510</t>
+  </si>
+  <si>
+    <t>BAB</t>
+  </si>
+  <si>
+    <t>BHS</t>
+  </si>
+  <si>
+    <t>EID</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>EUM</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GDO</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>GML</t>
+  </si>
+  <si>
+    <t>HEP</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>INS</t>
+  </si>
+  <si>
+    <t>IU</t>
+  </si>
+  <si>
+    <t>IUD</t>
+  </si>
+  <si>
+    <t>IUG</t>
+  </si>
+  <si>
+    <t>IUM</t>
+  </si>
+  <si>
+    <t>KIM</t>
+  </si>
+  <si>
+    <t>MEM</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>MGC</t>
+  </si>
+  <si>
+    <t>MGD</t>
+  </si>
+  <si>
+    <t>MGF</t>
+  </si>
+  <si>
+    <t>MGG</t>
+  </si>
+  <si>
+    <t>MGH</t>
+  </si>
+  <si>
+    <t>MGK</t>
+  </si>
+  <si>
+    <t>MGL</t>
+  </si>
+  <si>
+    <t>MGM</t>
+  </si>
+  <si>
+    <t>MGS</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>MIM</t>
+  </si>
+  <si>
+    <t>MIU</t>
+  </si>
+  <si>
+    <t>MJM</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MML</t>
+  </si>
+  <si>
+    <t>MMO</t>
+  </si>
+  <si>
+    <t>MOM</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>PDO</t>
+  </si>
+  <si>
+    <t>PER</t>
+  </si>
+  <si>
+    <t>PFU</t>
+  </si>
+  <si>
+    <t>PPM</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>RGD</t>
+  </si>
+  <si>
+    <t>RGG</t>
+  </si>
+  <si>
+    <t>RGH</t>
+  </si>
+  <si>
+    <t>RGM</t>
+  </si>
+  <si>
+    <t>RGT</t>
+  </si>
+  <si>
+    <t>RGV</t>
+  </si>
+  <si>
+    <t>RLM</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>SQM</t>
+  </si>
+  <si>
+    <t>SQV</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>TCI</t>
+  </si>
+  <si>
+    <t>UDO</t>
+  </si>
+  <si>
+    <t>UML</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>XAM</t>
+  </si>
+  <si>
+    <t>AUM</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -676,6 +679,9 @@
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -687,15 +693,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H1048576" totalsRowShown="0">
-  <autoFilter ref="A1:H1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I1048576" totalsRowShown="0">
+  <autoFilter ref="A1:I1048576"/>
   <sortState ref="A2:H64">
     <sortCondition ref="A1:A1048576"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" name=" strunut "/>
-    <tableColumn id="2" name="       streng        " dataDxfId="2"/>
-    <tableColumn id="3" name="Frequency" dataDxfId="1"/>
+    <tableColumn id="2" name="       streng        " dataDxfId="3"/>
+    <tableColumn id="3" name="Count" dataDxfId="2"/>
+    <tableColumn id="9" name="Frequency2" dataDxfId="1"/>
     <tableColumn id="4" name="Remark" dataDxfId="0"/>
     <tableColumn id="5" name="concept_id"/>
     <tableColumn id="6" name="concept_name"/>
@@ -969,26 +976,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,698 +1003,818 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
+        <v>110</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="C2" s="7">
         <v>7024</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>88444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>51</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7">
         <v>17</v>
       </c>
-      <c r="E8" s="1">
+      <c r="D8"/>
+      <c r="F8" s="1">
         <v>8695</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="2">
+        <v>8480</v>
+      </c>
+      <c r="I8" s="1">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C9" s="7">
         <v>458</v>
       </c>
-      <c r="E9" s="1">
+      <c r="D9">
+        <v>1226</v>
+      </c>
+      <c r="F9" s="1">
         <v>8504</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="1">
+        <v>8504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C10" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C11" s="7">
         <v>83</v>
       </c>
-      <c r="E11" s="1">
+      <c r="D11"/>
+      <c r="F11" s="1">
         <v>8636</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="1">
+        <v>8504</v>
+      </c>
+      <c r="I11">
+        <v>8519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C12" s="7">
         <v>13</v>
       </c>
-      <c r="E12" s="1">
+      <c r="D12"/>
+      <c r="F12" s="1">
         <v>9514</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="1">
+        <v>8504</v>
+      </c>
+      <c r="I12" s="1">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C13" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C14" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C15" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C16" s="7">
         <v>371</v>
       </c>
-      <c r="E16" s="1">
+      <c r="D16">
+        <v>1423</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="1">
         <v>8718</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="1">
+        <v>8718</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C17" s="7">
         <v>3</v>
       </c>
-      <c r="G17" s="1">
+      <c r="D17"/>
+      <c r="H17" s="1">
         <v>8718</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>45744809</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C18" s="7">
         <v>15</v>
       </c>
-      <c r="E18" s="1">
+      <c r="D18"/>
+      <c r="F18" s="1">
         <v>9333</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="1">
         <v>8718</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>8504</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C19" s="7">
         <v>486</v>
       </c>
-      <c r="E19" s="1">
+      <c r="D19">
+        <v>8821</v>
+      </c>
+      <c r="F19" s="1">
         <v>8985</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="1">
         <v>8718</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C20" s="7">
         <v>4</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="D20"/>
+      <c r="E20" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="1">
         <v>9525</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G20" s="6">
+      <c r="G20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="6">
         <v>8718</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C21" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C22" s="7">
         <v>18773</v>
       </c>
-      <c r="E22" s="1">
+      <c r="D22">
+        <v>676394</v>
+      </c>
+      <c r="F22" s="1">
         <v>8576</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="1">
+        <v>8576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C23" s="7">
         <v>2</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D23"/>
+      <c r="E23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="1">
         <v>9564</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="1">
         <v>8576</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C24" s="7">
         <v>211</v>
       </c>
-      <c r="E24" s="1">
+      <c r="D24">
+        <v>14134</v>
+      </c>
+      <c r="F24" s="1">
         <v>45890997</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="1">
         <v>8576</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>45744809</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C25" s="7">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D25">
+        <v>50</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="1">
         <v>45891022</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="1">
         <v>8576</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="2">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C26" s="7">
         <v>498</v>
       </c>
-      <c r="E26" s="1">
+      <c r="D26">
+        <v>9638</v>
+      </c>
+      <c r="F26" s="1">
         <v>8723</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="1">
+        <v>8576</v>
+      </c>
+      <c r="I26" s="1">
+        <v>8504</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>135</v>
       </c>
-      <c r="G26" s="1">
-        <v>8576</v>
-      </c>
-      <c r="H26" s="1">
-        <v>8504</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>50</v>
-      </c>
       <c r="B27" s="7" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C27" s="7">
         <v>102</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="D27">
+        <v>112</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="1">
         <v>8909</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="1">
         <v>8576</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>8512</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C28" s="7">
         <v>4</v>
       </c>
-      <c r="E28" s="1">
+      <c r="D28"/>
+      <c r="F28" s="1">
         <v>45891036</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="1">
         <v>8576</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>9483</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="E29" s="1">
+      <c r="D29"/>
+      <c r="F29" s="1">
         <v>8751</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="G29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="1">
         <v>8576</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>8519</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C30" s="7">
         <v>4797</v>
       </c>
-      <c r="E30" s="1">
+      <c r="D30">
+        <v>28584</v>
+      </c>
+      <c r="F30" s="1">
         <v>8861</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="1">
         <v>8576</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C31" s="7">
         <v>12</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D31"/>
+      <c r="E31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="1">
         <v>45891021</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G31" s="1">
+      <c r="G31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="1">
         <v>8576</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="2">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C32" s="7">
         <v>1</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D32"/>
+      <c r="E32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="1">
         <v>9040</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="1">
         <v>44777577</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>8519</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C33" s="7">
         <v>20</v>
       </c>
-      <c r="E33" s="1">
+      <c r="D33"/>
+      <c r="F33" s="1">
         <v>9550</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" s="1">
+      <c r="G33" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H33" s="1">
         <v>44777577</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="C34" s="7">
         <v>138</v>
       </c>
-      <c r="E34" s="1">
+      <c r="D34">
+        <v>10795</v>
+      </c>
+      <c r="F34" s="1">
         <v>44777577</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H34" s="1">
+        <v>44777577</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="C35" s="7">
         <v>338</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C36" s="7">
         <v>8</v>
       </c>
-      <c r="E36" s="1">
+      <c r="D36"/>
+      <c r="F36" s="1">
         <v>8587</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="1">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="C37" s="7">
         <v>8</v>
       </c>
-      <c r="E37" s="1">
+      <c r="D37"/>
+      <c r="F37" s="1">
         <v>8753</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G37" s="2">
+      <c r="G37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="2">
         <v>9573</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>8519</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="C38" s="7">
         <v>2</v>
       </c>
-      <c r="E38" s="1">
+      <c r="D38">
+        <v>2151</v>
+      </c>
+      <c r="F38" s="1">
         <v>9573</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H38" s="1">
+        <v>9573</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C39" s="7">
         <v>72</v>
       </c>
-      <c r="E39" s="1">
+      <c r="D39"/>
+      <c r="F39" s="1">
         <v>45891014</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G39" s="2">
+      <c r="G39" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" s="2">
         <v>9573</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="B40" s="8">
         <v>5.0000000000000001E-4</v>
@@ -1695,28 +1822,35 @@
       <c r="C40" s="7">
         <v>1433</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="1">
+      <c r="D40">
+        <v>21625</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="1">
         <v>8554</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="1">
+        <v>8554</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="C41" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="B42" s="9">
         <v>0.25</v>
@@ -1724,53 +1858,65 @@
       <c r="C42" s="7">
         <v>14</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="D42"/>
+      <c r="E42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="1">
         <v>8554</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H42" s="1">
+        <v>8554</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="C43" s="7">
         <v>1</v>
       </c>
-      <c r="E43" s="1">
+      <c r="D43"/>
+      <c r="F43" s="1">
         <v>9379</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="1">
+        <v>9379</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="C44" s="7">
         <v>4</v>
       </c>
-      <c r="E44" s="1">
+      <c r="D44"/>
+      <c r="F44" s="1">
         <v>9387</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="1">
+        <v>9387</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>84</v>
       </c>
       <c r="B45" s="9">
         <v>0.2</v>
@@ -1778,17 +1924,21 @@
       <c r="C45" s="7">
         <v>20</v>
       </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="1">
+      <c r="D45"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="1">
         <v>9234</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H45" s="1">
+        <v>9234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="B46" s="9">
         <v>0.08</v>
@@ -1796,312 +1946,387 @@
       <c r="C46" s="7">
         <v>4</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="1">
+      <c r="D46"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="1">
         <v>45891011</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H46" s="1">
+        <v>45891011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="C47" s="7">
         <v>512</v>
       </c>
-      <c r="E47" s="1">
+      <c r="D47">
+        <v>34928</v>
+      </c>
+      <c r="F47" s="1">
         <v>9655</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H47" s="1">
+        <v>9655</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="C48" s="7">
         <v>455</v>
       </c>
-      <c r="E48" s="1">
+      <c r="D48">
+        <v>22006</v>
+      </c>
+      <c r="F48" s="1">
         <v>45890998</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G48" s="1">
+      <c r="G48" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H48" s="1">
         <v>9655</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48">
+        <v>45744809</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="C49" s="7">
         <v>39</v>
       </c>
-      <c r="E49" s="1">
+      <c r="D49">
+        <v>274</v>
+      </c>
+      <c r="F49" s="1">
         <v>8720</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="1">
         <v>9655</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <v>8504</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="C50" s="7">
         <v>67</v>
       </c>
-      <c r="E50" s="1">
+      <c r="D50">
+        <v>596</v>
+      </c>
+      <c r="F50" s="1">
         <v>8906</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G50" s="1">
+      <c r="G50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="1">
         <v>9655</v>
       </c>
-      <c r="H50" s="2">
+      <c r="I50" s="2">
         <v>8512</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C51" s="7">
         <v>227</v>
       </c>
-      <c r="E51" s="1">
+      <c r="D51">
+        <v>3942</v>
+      </c>
+      <c r="F51" s="1">
         <v>8859</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G51" s="1">
+      <c r="G51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51" s="1">
         <v>9655</v>
       </c>
-      <c r="H51" s="1">
+      <c r="I51" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="C52" s="7">
         <v>144</v>
       </c>
-      <c r="E52" s="1">
+      <c r="D52">
+        <v>3181</v>
+      </c>
+      <c r="F52" s="1">
         <v>44777645</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G52" s="1">
+      <c r="G52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H52" s="1">
         <v>9655</v>
       </c>
-      <c r="H52" s="2">
+      <c r="I52" s="2">
         <v>8505</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>161</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="C53" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="C54" s="7">
         <v>1</v>
       </c>
-      <c r="E54" s="1">
+      <c r="D54"/>
+      <c r="F54" s="1">
         <v>45891029</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G54" s="2">
+      <c r="G54" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H54" s="2">
         <v>9665</v>
       </c>
-      <c r="H54" s="1">
+      <c r="I54" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="C55" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="C56" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <v>136</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="C57" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="C58" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <v>62</v>
+      </c>
+      <c r="F58" s="1">
+        <v>8576</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H58" s="1">
+        <v>8576</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="C59" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="C60" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>169</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
       <c r="C61" s="7">
         <v>65</v>
       </c>
-      <c r="E61" s="1">
+      <c r="D61">
+        <v>5431</v>
+      </c>
+      <c r="F61" s="1">
         <v>8763</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G61" s="1">
+      <c r="G61" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" s="1">
         <v>8510</v>
       </c>
-      <c r="H61" s="1">
+      <c r="I61" s="1">
         <v>8587</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>170</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="C62" s="7">
         <v>35</v>
       </c>
-      <c r="E62" s="1">
+      <c r="D62"/>
+      <c r="F62" s="1">
         <v>8510</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G62" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H62" s="1">
+        <v>8510</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="C63" s="7">
         <v>108</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63"/>
+      <c r="F63" s="1">
+        <v>8523</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H63" s="1">
+        <v>8523</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>172</v>
       </c>
-      <c r="E63" s="1">
-        <v>8523</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>120</v>
-      </c>
       <c r="B64" s="7" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="C64" s="7">
         <v>133</v>
+      </c>
+      <c r="D64">
+        <v>28</v>
+      </c>
+      <c r="F64" s="1">
+        <v>8985</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H64" s="1">
+        <v>8718</v>
+      </c>
+      <c r="I64" s="1">
+        <v>8587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>